<commit_message>
new boiling_plan format parse boiling_params
</commit_message>
<xml_diff>
--- a/app/schedule_maker/data/sample_boiling_plan.xlsx
+++ b/app/schedule_maker/data/sample_boiling_plan.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Levkina\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mi\Desktop\code\git\2020.10-umalat\umalat\app\schedule_maker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6A0306-3E0C-4AF3-8B63-EF8C2E131D25}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6470" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Вода" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
   <definedNames>
     <definedName name="Water_SKU">'Вода SKU'!$A$1:$A$100</definedName>
   </definedNames>
-  <calcPr calcId="162913" refMode="R1C1"/>
+  <calcPr calcId="179021" refMode="R1C1"/>
 </workbook>
 </file>
 
@@ -72,9 +73,6 @@
     <t>-</t>
   </si>
   <si>
-    <t xml:space="preserve">3.3 Сакко </t>
-  </si>
-  <si>
     <t>Моцарелла Фиор Ди Латте в воде "Pretto", 45%, 0,125 кг, ф/п, (8 шт)</t>
   </si>
   <si>
@@ -94,9 +92,6 @@
   </si>
   <si>
     <t>Моцарелла в воде Фиор Ди Латте "Каждый день", 45%, 0,1 кг, ф/п</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.6 Альче </t>
   </si>
   <si>
     <t>Моцарелла Грандиоза в воде "Unagrande", 50%, 0,2 кг, ф/п</t>
@@ -123,9 +118,6 @@
     <t>Моцарелла Чильеджина в воде "Ваш выбор", 50%, 0,1 кг, ф/п</t>
   </si>
   <si>
-    <t xml:space="preserve">2.7 Альче </t>
-  </si>
-  <si>
     <t>Для пиццы</t>
   </si>
   <si>
@@ -136,9 +128,6 @@
   </si>
   <si>
     <t>Сулугуни "Умалат" (для хачапури), 45%, 0,12 кг, ф/п</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.7 Сакко </t>
   </si>
   <si>
     <t>Моцарелла "Pretto" (для бутербродов), 45%, 0,2 кг, т/ф, (9 шт)</t>
@@ -251,11 +240,23 @@
   <si>
     <t>Сулугуни палочки "Умалат", 45%, 0,12 кг, т/ф (10 шт.)</t>
   </si>
+  <si>
+    <t xml:space="preserve">2.7, Сакко </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.7, Альче </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.3, Сакко </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.6, Альче </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -361,7 +362,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
@@ -785,33 +786,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK116"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="13" ySplit="1" topLeftCell="N17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="13" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="N1" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.6328125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.6640625" style="1" customWidth="1"/>
     <col min="3" max="4" width="15" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.36328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="37.7265625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="37.77734375" style="1" customWidth="1"/>
     <col min="7" max="7" width="15" style="1" customWidth="1"/>
-    <col min="8" max="9" width="8.7265625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="1.7265625" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="8.77734375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="1.77734375" style="1" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="2" style="1" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="1.6328125" style="1" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="2.54296875" style="1" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="7.26953125" style="1" hidden="1" customWidth="1"/>
-    <col min="15" max="1025" width="8.54296875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="1.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="2.5546875" style="1" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="7.21875" style="1" hidden="1" customWidth="1"/>
+    <col min="15" max="1025" width="8.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -852,7 +853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <f t="shared" ref="A2:A21" ca="1" si="0">IF(J2="-", "", 1 + 80 + SUM(INDIRECT(ADDRESS(2,COLUMN(M2)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(M2)))))</f>
         <v>81</v>
@@ -862,7 +863,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="D2" s="4">
         <v>1000</v>
@@ -871,7 +872,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" s="4">
         <v>99</v>
@@ -900,7 +901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <f t="shared" ca="1" si="0"/>
         <v>81</v>
@@ -910,7 +911,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="D3" s="4">
         <v>1000</v>
@@ -919,7 +920,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" s="4">
         <v>302</v>
@@ -948,7 +949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <f t="shared" ca="1" si="0"/>
         <v>81</v>
@@ -958,7 +959,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="D4" s="4">
         <v>1000</v>
@@ -967,7 +968,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" s="4">
         <v>33</v>
@@ -996,7 +997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <f t="shared" ca="1" si="0"/>
         <v>81</v>
@@ -1006,7 +1007,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="D5" s="4">
         <v>1000</v>
@@ -1015,7 +1016,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" s="4">
         <v>243</v>
@@ -1044,7 +1045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <f t="shared" ca="1" si="0"/>
         <v>81</v>
@@ -1054,7 +1055,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="D6" s="4">
         <v>1000</v>
@@ -1063,7 +1064,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G6" s="4">
         <v>103</v>
@@ -1092,7 +1093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <f t="shared" ca="1" si="0"/>
         <v>81</v>
@@ -1102,7 +1103,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="D7" s="4">
         <v>1000</v>
@@ -1111,7 +1112,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G7" s="4">
         <v>53</v>
@@ -1140,7 +1141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <f t="shared" ca="1" si="0"/>
         <v>81</v>
@@ -1150,7 +1151,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="D8" s="4">
         <v>1000</v>
@@ -1159,7 +1160,7 @@
         <v>12</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G8" s="4">
         <v>167</v>
@@ -1188,7 +1189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
@@ -1239,7 +1240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <f t="shared" ca="1" si="0"/>
         <v>82</v>
@@ -1249,7 +1250,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="D10" s="4">
         <v>1000</v>
@@ -1258,7 +1259,7 @@
         <v>12</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G10" s="4">
         <v>26</v>
@@ -1287,7 +1288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <f t="shared" ca="1" si="0"/>
         <v>82</v>
@@ -1297,7 +1298,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="D11" s="4">
         <v>1000</v>
@@ -1306,7 +1307,7 @@
         <v>12</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G11" s="4">
         <v>974</v>
@@ -1335,7 +1336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
@@ -1386,7 +1387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
         <f t="shared" ca="1" si="0"/>
         <v>83</v>
@@ -1395,17 +1396,17 @@
         <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>23</v>
+      <c r="C13" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="D13" s="12">
         <v>1000</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G13" s="12">
         <v>1000</v>
@@ -1434,7 +1435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
@@ -1485,7 +1486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <f t="shared" ca="1" si="0"/>
         <v>84</v>
@@ -1494,17 +1495,17 @@
         <f t="shared" ca="1" si="1"/>
         <v>4</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>23</v>
+      <c r="C15" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="D15" s="12">
         <v>1000</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G15" s="12">
         <v>1000</v>
@@ -1533,7 +1534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
@@ -1584,7 +1585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <f t="shared" ca="1" si="0"/>
         <v>85</v>
@@ -1593,17 +1594,17 @@
         <f t="shared" ca="1" si="1"/>
         <v>5</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>15</v>
+      <c r="C17" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="D17" s="12">
         <v>1000</v>
       </c>
       <c r="E17" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="12" t="s">
         <v>26</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="G17" s="12">
         <v>679</v>
@@ -1632,7 +1633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <f t="shared" ca="1" si="0"/>
         <v>85</v>
@@ -1641,17 +1642,17 @@
         <f t="shared" ca="1" si="1"/>
         <v>5</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>15</v>
+      <c r="C18" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="D18" s="12">
         <v>1000</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G18" s="12">
         <v>28</v>
@@ -1680,7 +1681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10">
         <f t="shared" ca="1" si="0"/>
         <v>85</v>
@@ -1689,17 +1690,17 @@
         <f t="shared" ca="1" si="1"/>
         <v>5</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>15</v>
+      <c r="C19" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="D19" s="12">
         <v>1000</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G19" s="12">
         <v>198</v>
@@ -1728,7 +1729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
         <f t="shared" ca="1" si="0"/>
         <v>85</v>
@@ -1737,17 +1738,17 @@
         <f t="shared" ca="1" si="1"/>
         <v>5</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>15</v>
+      <c r="C20" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="D20" s="12">
         <v>1000</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G20" s="12">
         <v>95</v>
@@ -1776,7 +1777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
@@ -1827,7 +1828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13"/>
       <c r="B22" s="8" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1854,7 +1855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13"/>
       <c r="B23" s="8" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1881,7 +1882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13"/>
       <c r="B24" s="8" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1908,7 +1909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13"/>
       <c r="B25" s="8" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1935,7 +1936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13"/>
       <c r="B26" s="8" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1962,7 +1963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13"/>
       <c r="B27" s="8" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1989,7 +1990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13"/>
       <c r="B28" s="8" t="str">
         <f t="shared" ref="B28:B59" ca="1" si="7">IF(F28="","",IF(J28="-","",1+SUM(INDIRECT(ADDRESS(2,COLUMN(M28))&amp;":"&amp;ADDRESS(ROW(),COLUMN(M28))))))</f>
@@ -2016,7 +2017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13"/>
       <c r="B29" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -2043,7 +2044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13"/>
       <c r="B30" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -2070,7 +2071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="13"/>
       <c r="B31" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -2097,7 +2098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="13"/>
       <c r="B32" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -2124,7 +2125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13"/>
       <c r="B33" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -2151,7 +2152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13"/>
       <c r="B34" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -2178,7 +2179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="13"/>
       <c r="B35" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -2205,7 +2206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13"/>
       <c r="B36" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -2232,7 +2233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="13"/>
       <c r="B37" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -2259,7 +2260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="13"/>
       <c r="B38" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -2286,7 +2287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="13"/>
       <c r="B39" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -2313,7 +2314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="13"/>
       <c r="B40" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -2340,7 +2341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="13"/>
       <c r="B41" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -2367,7 +2368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="13"/>
       <c r="B42" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -2394,7 +2395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
         <v/>
@@ -2420,7 +2421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
         <v/>
@@ -2446,7 +2447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
         <v/>
@@ -2472,7 +2473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
         <v/>
@@ -2498,7 +2499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
         <v/>
@@ -2524,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
         <v/>
@@ -2550,7 +2551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
         <v/>
@@ -2576,7 +2577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
         <v/>
@@ -2602,7 +2603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
         <v/>
@@ -2628,7 +2629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
         <v/>
@@ -2654,7 +2655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
         <v/>
@@ -2680,7 +2681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
         <v/>
@@ -2706,7 +2707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
         <v/>
@@ -2732,7 +2733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
         <v/>
@@ -2758,7 +2759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
         <v/>
@@ -2784,7 +2785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
         <v/>
@@ -2810,7 +2811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="8" t="str">
         <f t="shared" ca="1" si="7"/>
         <v/>
@@ -2836,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="8" t="str">
         <f t="shared" ref="B60:B71" ca="1" si="13">IF(F60="","",IF(J60="-","",1+SUM(INDIRECT(ADDRESS(2,COLUMN(M60))&amp;":"&amp;ADDRESS(ROW(),COLUMN(M60))))))</f>
         <v/>
@@ -2862,7 +2863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="8" t="str">
         <f t="shared" ca="1" si="13"/>
         <v/>
@@ -2888,7 +2889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="8" t="str">
         <f t="shared" ca="1" si="13"/>
         <v/>
@@ -2914,7 +2915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="8" t="str">
         <f t="shared" ca="1" si="13"/>
         <v/>
@@ -2940,7 +2941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="8" t="str">
         <f t="shared" ca="1" si="13"/>
         <v/>
@@ -2966,7 +2967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="8" t="str">
         <f t="shared" ca="1" si="13"/>
         <v/>
@@ -2992,7 +2993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="8" t="str">
         <f t="shared" ca="1" si="13"/>
         <v/>
@@ -3018,7 +3019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="8" t="str">
         <f t="shared" ca="1" si="13"/>
         <v/>
@@ -3044,7 +3045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="8" t="str">
         <f t="shared" ca="1" si="13"/>
         <v/>
@@ -3070,7 +3071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="8" t="str">
         <f t="shared" ca="1" si="13"/>
         <v/>
@@ -3096,7 +3097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="8" t="str">
         <f t="shared" ca="1" si="13"/>
         <v/>
@@ -3122,7 +3123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B71" s="8" t="str">
         <f t="shared" ca="1" si="13"/>
         <v/>
@@ -3148,7 +3149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H72" s="1" t="str">
         <f t="shared" ca="1" si="14"/>
         <v/>
@@ -3170,7 +3171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H73" s="1" t="str">
         <f t="shared" ca="1" si="14"/>
         <v/>
@@ -3192,7 +3193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H74" s="1" t="str">
         <f t="shared" ca="1" si="14"/>
         <v/>
@@ -3214,7 +3215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H75" s="1" t="str">
         <f t="shared" ca="1" si="14"/>
         <v/>
@@ -3236,7 +3237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H76" s="1" t="str">
         <f t="shared" ca="1" si="14"/>
         <v/>
@@ -3258,7 +3259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H77" s="1" t="str">
         <f t="shared" ca="1" si="14"/>
         <v/>
@@ -3280,7 +3281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H78" s="1" t="str">
         <f t="shared" ca="1" si="14"/>
         <v/>
@@ -3302,7 +3303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H79" s="1" t="str">
         <f t="shared" ca="1" si="14"/>
         <v/>
@@ -3324,7 +3325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H80" s="1" t="str">
         <f t="shared" ca="1" si="14"/>
         <v/>
@@ -3346,7 +3347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H81" s="1" t="str">
         <f t="shared" ca="1" si="14"/>
         <v/>
@@ -3368,7 +3369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H82" s="1" t="str">
         <f t="shared" ca="1" si="14"/>
         <v/>
@@ -3390,7 +3391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H83" s="1" t="str">
         <f t="shared" ca="1" si="14"/>
         <v/>
@@ -3412,7 +3413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H84" s="1" t="str">
         <f t="shared" ca="1" si="14"/>
         <v/>
@@ -3434,7 +3435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H85" s="1" t="str">
         <f t="shared" ca="1" si="14"/>
         <v/>
@@ -3456,7 +3457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H86" s="1" t="str">
         <f t="shared" ca="1" si="14"/>
         <v/>
@@ -3478,7 +3479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H87" s="1" t="str">
         <f t="shared" ca="1" si="14"/>
         <v/>
@@ -3500,7 +3501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H88" s="1" t="str">
         <f t="shared" ca="1" si="14"/>
         <v/>
@@ -3522,7 +3523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H89" s="1" t="str">
         <f t="shared" ca="1" si="14"/>
         <v/>
@@ -3544,7 +3545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H90" s="1" t="str">
         <f t="shared" ca="1" si="14"/>
         <v/>
@@ -3566,7 +3567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H91" s="1" t="str">
         <f t="shared" ca="1" si="14"/>
         <v/>
@@ -3588,7 +3589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H92" s="1" t="str">
         <f t="shared" ref="H92:H116" ca="1" si="21">IF(N92 - INDIRECT("N" &amp; ROW() - 1) = 0, "", INDIRECT("N" &amp; ROW() - 1) - N92)</f>
         <v/>
@@ -3610,7 +3611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H93" s="1" t="str">
         <f t="shared" ca="1" si="21"/>
         <v/>
@@ -3632,7 +3633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H94" s="1" t="str">
         <f t="shared" ca="1" si="21"/>
         <v/>
@@ -3654,7 +3655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H95" s="1" t="str">
         <f t="shared" ca="1" si="21"/>
         <v/>
@@ -3676,7 +3677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H96" s="1" t="str">
         <f t="shared" ca="1" si="21"/>
         <v/>
@@ -3698,7 +3699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H97" s="1" t="str">
         <f t="shared" ca="1" si="21"/>
         <v/>
@@ -3720,7 +3721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H98" s="1" t="str">
         <f t="shared" ca="1" si="21"/>
         <v/>
@@ -3742,7 +3743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H99" s="1" t="str">
         <f t="shared" ca="1" si="21"/>
         <v/>
@@ -3764,7 +3765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H100" s="1" t="str">
         <f t="shared" ca="1" si="21"/>
         <v/>
@@ -3786,7 +3787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H101" s="1" t="str">
         <f t="shared" ca="1" si="21"/>
         <v/>
@@ -3808,7 +3809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H102" s="1" t="str">
         <f t="shared" ca="1" si="21"/>
         <v/>
@@ -3830,7 +3831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H103" s="1" t="str">
         <f t="shared" ca="1" si="21"/>
         <v/>
@@ -3852,7 +3853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H104" s="1" t="str">
         <f t="shared" ca="1" si="21"/>
         <v/>
@@ -3874,7 +3875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H105" s="1" t="str">
         <f t="shared" ca="1" si="21"/>
         <v/>
@@ -3896,7 +3897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H106" s="1" t="str">
         <f t="shared" ca="1" si="21"/>
         <v/>
@@ -3918,7 +3919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H107" s="1" t="str">
         <f t="shared" ca="1" si="21"/>
         <v/>
@@ -3940,7 +3941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H108" s="1" t="str">
         <f t="shared" ca="1" si="21"/>
         <v/>
@@ -3962,7 +3963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H109" s="1" t="str">
         <f t="shared" ca="1" si="21"/>
         <v/>
@@ -3984,7 +3985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H110" s="1" t="str">
         <f t="shared" ca="1" si="21"/>
         <v/>
@@ -4006,7 +4007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H111" s="1" t="str">
         <f t="shared" ca="1" si="21"/>
         <v/>
@@ -4028,7 +4029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H112" s="1" t="str">
         <f t="shared" ca="1" si="21"/>
         <v/>
@@ -4050,7 +4051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H113" s="1" t="str">
         <f t="shared" ca="1" si="21"/>
         <v/>
@@ -4072,7 +4073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H114" s="1" t="str">
         <f t="shared" ca="1" si="21"/>
         <v/>
@@ -4094,7 +4095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H115" s="1" t="str">
         <f t="shared" ca="1" si="21"/>
         <v/>
@@ -4116,7 +4117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H116" s="1" t="str">
         <f t="shared" ca="1" si="21"/>
         <v/>
@@ -4154,7 +4155,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>'Вода SKU'!$A$1:$A$137</xm:f>
           </x14:formula1>
@@ -4170,33 +4171,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK123"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="13" ySplit="1" topLeftCell="N5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="13" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="N1" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.6328125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.6640625" style="1" customWidth="1"/>
     <col min="3" max="4" width="15" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.36328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="37.7265625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="37.77734375" style="1" customWidth="1"/>
     <col min="7" max="7" width="15" style="1" customWidth="1"/>
-    <col min="8" max="9" width="8.7265625" style="1" customWidth="1"/>
+    <col min="8" max="9" width="8.77734375" style="1" customWidth="1"/>
     <col min="10" max="10" width="3" style="1" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="1" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="4" style="1" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="3.81640625" style="1" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="8.26953125" style="1" hidden="1" customWidth="1"/>
-    <col min="15" max="1025" width="8.54296875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="3.77734375" style="1" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="8.21875" style="1" hidden="1" customWidth="1"/>
+    <col min="15" max="1025" width="8.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="20.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4237,7 +4238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19">
         <f ca="1">IF(J2="-", "-", 1 + MAX(Вода!$A$2:$A$94) + 80 + SUM(INDIRECT(ADDRESS(2,COLUMN(M2)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(M2)))))</f>
         <v>166</v>
@@ -4247,16 +4248,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="D2" s="14">
         <v>850</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G2" s="14">
         <v>850</v>
@@ -4285,7 +4286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="str">
         <f ca="1">IF(J3="-", "-", 1 + MAX(Вода!$A$2:$A$94) + 80 + SUM(INDIRECT(ADDRESS(2,COLUMN(M3)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(M3)))))</f>
         <v>-</v>
@@ -4336,7 +4337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19">
         <f ca="1">IF(J4="-", "-", 1 + MAX(Вода!$A$2:$A$94) + 80 + SUM(INDIRECT(ADDRESS(2,COLUMN(M4)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(M4)))))</f>
         <v>167</v>
@@ -4346,16 +4347,16 @@
         <v>2</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="D4" s="14">
         <v>850</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G4" s="14">
         <v>850</v>
@@ -4384,7 +4385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="str">
         <f ca="1">IF(J5="-", "-", 1 + MAX(Вода!$A$2:$A$94) + 80 + SUM(INDIRECT(ADDRESS(2,COLUMN(M5)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(M5)))))</f>
         <v>-</v>
@@ -4435,7 +4436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19">
         <f ca="1">IF(J6="-", "-", 1 + MAX(Вода!$A$2:$A$94) + 80 + SUM(INDIRECT(ADDRESS(2,COLUMN(M6)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(M6)))))</f>
         <v>168</v>
@@ -4445,16 +4446,16 @@
         <v>3</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="D6" s="14">
         <v>850</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G6" s="14">
         <v>850</v>
@@ -4483,7 +4484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="str">
         <f ca="1">IF(J7="-", "-", 1 + MAX(Вода!$A$2:$A$94) + 80 + SUM(INDIRECT(ADDRESS(2,COLUMN(M7)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(M7)))))</f>
         <v>-</v>
@@ -4534,7 +4535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19">
         <f ca="1">IF(J8="-", "-", 1 + MAX(Вода!$A$2:$A$94) + 80 + SUM(INDIRECT(ADDRESS(2,COLUMN(M8)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(M8)))))</f>
         <v>169</v>
@@ -4544,16 +4545,16 @@
         <v>4</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="D8" s="14">
         <v>850</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G8" s="14">
         <v>850</v>
@@ -4582,7 +4583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="str">
         <f ca="1">IF(J9="-", "-", 1 + MAX(Вода!$A$2:$A$94) + 80 + SUM(INDIRECT(ADDRESS(2,COLUMN(M9)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(M9)))))</f>
         <v>-</v>
@@ -4633,7 +4634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19">
         <f ca="1">IF(J10="-", "-", 1 + MAX(Вода!$A$2:$A$94) + 80 + SUM(INDIRECT(ADDRESS(2,COLUMN(M10)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(M10)))))</f>
         <v>170</v>
@@ -4643,16 +4644,16 @@
         <v>5</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="D10" s="14">
         <v>850</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G10" s="14">
         <v>850</v>
@@ -4681,7 +4682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="str">
         <f ca="1">IF(J11="-", "-", 1 + MAX(Вода!$A$2:$A$94) + 80 + SUM(INDIRECT(ADDRESS(2,COLUMN(M11)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(M11)))))</f>
         <v>-</v>
@@ -4732,7 +4733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19">
         <f ca="1">IF(J12="-", "-", 1 + MAX(Вода!$A$2:$A$94) + 80 + SUM(INDIRECT(ADDRESS(2,COLUMN(M12)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(M12)))))</f>
         <v>171</v>
@@ -4742,16 +4743,16 @@
         <v>6</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="D12" s="14">
         <v>850</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G12" s="14">
         <v>842</v>
@@ -4780,7 +4781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
         <f ca="1">IF(J13="-", "-", 1 + MAX(Вода!$A$2:$A$94) + 80 + SUM(INDIRECT(ADDRESS(2,COLUMN(M13)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(M13)))))</f>
         <v>171</v>
@@ -4790,16 +4791,16 @@
         <v>6</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="D13" s="14">
         <v>850</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G13" s="14">
         <v>8</v>
@@ -4828,7 +4829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" s="1" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="str">
         <f ca="1">IF(J14="-", "-", 1 + MAX(Вода!$A$2:$A$94) + 80 + SUM(INDIRECT(ADDRESS(2,COLUMN(M14)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(M14)))))</f>
         <v>-</v>
@@ -4879,7 +4880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" s="1" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <f ca="1">IF(J15="-", "-", 1 + MAX(Вода!$A$2:$A$94) + 80 + SUM(INDIRECT(ADDRESS(2,COLUMN(M15)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(M15)))))</f>
         <v>172</v>
@@ -4889,16 +4890,16 @@
         <v>7</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="D15" s="14">
         <v>850</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G15" s="14">
         <v>850</v>
@@ -4927,7 +4928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" s="1" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="str">
         <f ca="1">IF(J16="-", "-", 1 + MAX(Вода!$A$2:$A$94) + 80 + SUM(INDIRECT(ADDRESS(2,COLUMN(M16)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(M16)))))</f>
         <v>-</v>
@@ -4978,7 +4979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16">
         <f ca="1">IF(J17="-", "-", 1 + MAX(Вода!$A$2:$A$94) + 80 + SUM(INDIRECT(ADDRESS(2,COLUMN(M17)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(M17)))))</f>
         <v>173</v>
@@ -4988,16 +4989,16 @@
         <v>8</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="D17" s="18">
         <v>850</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G17" s="18">
         <v>850</v>
@@ -5026,7 +5027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="str">
         <f ca="1">IF(J18="-", "-", 1 + MAX(Вода!$A$2:$A$94) + 80 + SUM(INDIRECT(ADDRESS(2,COLUMN(M18)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(M18)))))</f>
         <v>-</v>
@@ -5077,7 +5078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16">
         <f ca="1">IF(J19="-", "-", 1 + MAX(Вода!$A$2:$A$94) + 80 + SUM(INDIRECT(ADDRESS(2,COLUMN(M19)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(M19)))))</f>
         <v>174</v>
@@ -5087,16 +5088,16 @@
         <v>9</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="D19" s="18">
         <v>850</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G19" s="18">
         <v>659</v>
@@ -5125,7 +5126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16">
         <f ca="1">IF(J20="-", "-", 1 + MAX(Вода!$A$2:$A$94) + 80 + SUM(INDIRECT(ADDRESS(2,COLUMN(M20)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(M20)))))</f>
         <v>174</v>
@@ -5135,16 +5136,16 @@
         <v>9</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="D20" s="18">
         <v>850</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G20" s="18">
         <v>191</v>
@@ -5173,7 +5174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="str">
         <f ca="1">IF(J21="-", "-", 1 + MAX(Вода!$A$2:$A$94) + 80 + SUM(INDIRECT(ADDRESS(2,COLUMN(M21)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(M21)))))</f>
         <v>-</v>
@@ -5224,7 +5225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13"/>
       <c r="B22" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -5251,7 +5252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13"/>
       <c r="B23" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -5278,7 +5279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13"/>
       <c r="B24" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -5305,7 +5306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13"/>
       <c r="B25" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -5332,7 +5333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13"/>
       <c r="B26" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -5359,7 +5360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13"/>
       <c r="B27" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -5386,7 +5387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13"/>
       <c r="B28" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -5413,7 +5414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13"/>
       <c r="B29" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -5440,7 +5441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13"/>
       <c r="B30" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -5467,7 +5468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="13"/>
       <c r="B31" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -5494,7 +5495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="13"/>
       <c r="B32" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -5521,7 +5522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13"/>
       <c r="B33" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -5548,7 +5549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13"/>
       <c r="B34" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -5575,7 +5576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="13"/>
       <c r="B35" s="8" t="str">
         <f t="shared" ref="B35:B66" ca="1" si="18">IF(F35="","",IF(J35="-","",1+SUM(INDIRECT(ADDRESS(2,COLUMN(M35))&amp;":"&amp;ADDRESS(ROW(),COLUMN(M35))))))</f>
@@ -5602,7 +5603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13"/>
       <c r="B36" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
@@ -5629,7 +5630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="13"/>
       <c r="B37" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
@@ -5656,7 +5657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="13"/>
       <c r="B38" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
@@ -5683,7 +5684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="13"/>
       <c r="B39" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
@@ -5710,7 +5711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="13"/>
       <c r="B40" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
@@ -5737,7 +5738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="13"/>
       <c r="B41" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
@@ -5764,7 +5765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="13"/>
       <c r="B42" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
@@ -5791,7 +5792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="13"/>
       <c r="B43" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
@@ -5818,7 +5819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="13"/>
       <c r="B44" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
@@ -5845,7 +5846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="13"/>
       <c r="B45" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
@@ -5872,7 +5873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="13"/>
       <c r="B46" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
@@ -5899,7 +5900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="13"/>
       <c r="B47" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
@@ -5926,7 +5927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="13"/>
       <c r="B48" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
@@ -5953,7 +5954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="13"/>
       <c r="B49" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
@@ -5980,7 +5981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
         <v/>
@@ -6006,7 +6007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
         <v/>
@@ -6032,7 +6033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
         <v/>
@@ -6058,7 +6059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
         <v/>
@@ -6084,7 +6085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
         <v/>
@@ -6110,7 +6111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
         <v/>
@@ -6136,7 +6137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
         <v/>
@@ -6162,7 +6163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
         <v/>
@@ -6188,7 +6189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
         <v/>
@@ -6214,7 +6215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
         <v/>
@@ -6240,7 +6241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
         <v/>
@@ -6266,7 +6267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
         <v/>
@@ -6292,7 +6293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
         <v/>
@@ -6318,7 +6319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
         <v/>
@@ -6344,7 +6345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
         <v/>
@@ -6370,7 +6371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
         <v/>
@@ -6396,7 +6397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="8" t="str">
         <f t="shared" ca="1" si="18"/>
         <v/>
@@ -6422,7 +6423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="8" t="str">
         <f t="shared" ref="B67:B78" ca="1" si="24">IF(F67="","",IF(J67="-","",1+SUM(INDIRECT(ADDRESS(2,COLUMN(M67))&amp;":"&amp;ADDRESS(ROW(),COLUMN(M67))))))</f>
         <v/>
@@ -6448,7 +6449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="8" t="str">
         <f t="shared" ca="1" si="24"/>
         <v/>
@@ -6474,7 +6475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="8" t="str">
         <f t="shared" ca="1" si="24"/>
         <v/>
@@ -6500,7 +6501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="8" t="str">
         <f t="shared" ca="1" si="24"/>
         <v/>
@@ -6526,7 +6527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B71" s="8" t="str">
         <f t="shared" ca="1" si="24"/>
         <v/>
@@ -6552,7 +6553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B72" s="8" t="str">
         <f t="shared" ca="1" si="24"/>
         <v/>
@@ -6578,7 +6579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73" s="8" t="str">
         <f t="shared" ca="1" si="24"/>
         <v/>
@@ -6604,7 +6605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="8" t="str">
         <f t="shared" ca="1" si="24"/>
         <v/>
@@ -6630,7 +6631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B75" s="8" t="str">
         <f t="shared" ca="1" si="24"/>
         <v/>
@@ -6656,7 +6657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B76" s="8" t="str">
         <f t="shared" ca="1" si="24"/>
         <v/>
@@ -6682,7 +6683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B77" s="8" t="str">
         <f t="shared" ca="1" si="24"/>
         <v/>
@@ -6708,7 +6709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B78" s="8" t="str">
         <f t="shared" ca="1" si="24"/>
         <v/>
@@ -6734,7 +6735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H79" s="1" t="str">
         <f t="shared" ca="1" si="31"/>
         <v/>
@@ -6756,7 +6757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H80" s="1" t="str">
         <f t="shared" ca="1" si="31"/>
         <v/>
@@ -6778,7 +6779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H81" s="1" t="str">
         <f t="shared" ca="1" si="31"/>
         <v/>
@@ -6800,7 +6801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H82" s="1" t="str">
         <f t="shared" ca="1" si="31"/>
         <v/>
@@ -6822,7 +6823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H83" s="1" t="str">
         <f t="shared" ca="1" si="31"/>
         <v/>
@@ -6844,7 +6845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H84" s="1" t="str">
         <f t="shared" ca="1" si="31"/>
         <v/>
@@ -6866,7 +6867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H85" s="1" t="str">
         <f t="shared" ca="1" si="31"/>
         <v/>
@@ -6888,7 +6889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H86" s="1" t="str">
         <f t="shared" ca="1" si="31"/>
         <v/>
@@ -6910,7 +6911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H87" s="1" t="str">
         <f t="shared" ca="1" si="31"/>
         <v/>
@@ -6932,7 +6933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H88" s="1" t="str">
         <f t="shared" ca="1" si="31"/>
         <v/>
@@ -6954,7 +6955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H89" s="1" t="str">
         <f t="shared" ca="1" si="31"/>
         <v/>
@@ -6976,7 +6977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H90" s="1" t="str">
         <f t="shared" ca="1" si="31"/>
         <v/>
@@ -6998,7 +6999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H91" s="1" t="str">
         <f t="shared" ca="1" si="31"/>
         <v/>
@@ -7020,7 +7021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H92" s="1" t="str">
         <f t="shared" ca="1" si="31"/>
         <v/>
@@ -7042,7 +7043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H93" s="1" t="str">
         <f t="shared" ca="1" si="31"/>
         <v/>
@@ -7064,7 +7065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H94" s="1" t="str">
         <f t="shared" ca="1" si="31"/>
         <v/>
@@ -7086,7 +7087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H95" s="1" t="str">
         <f t="shared" ca="1" si="31"/>
         <v/>
@@ -7108,7 +7109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H96" s="1" t="str">
         <f t="shared" ca="1" si="31"/>
         <v/>
@@ -7130,7 +7131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H97" s="1" t="str">
         <f t="shared" ca="1" si="31"/>
         <v/>
@@ -7152,7 +7153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H98" s="1" t="str">
         <f t="shared" ca="1" si="31"/>
         <v/>
@@ -7174,7 +7175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H99" s="1" t="str">
         <f t="shared" ca="1" si="31"/>
         <v/>
@@ -7196,7 +7197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H100" s="1" t="str">
         <f t="shared" ca="1" si="31"/>
         <v/>
@@ -7218,7 +7219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H101" s="1" t="str">
         <f t="shared" ref="H101:H123" ca="1" si="35">IF(N101 - INDIRECT("N" &amp; ROW() - 1) = 0, "", INDIRECT("N" &amp; ROW() - 1) - N101)</f>
         <v/>
@@ -7240,7 +7241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H102" s="1" t="str">
         <f t="shared" ca="1" si="35"/>
         <v/>
@@ -7262,7 +7263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H103" s="1" t="str">
         <f t="shared" ca="1" si="35"/>
         <v/>
@@ -7284,7 +7285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H104" s="1" t="str">
         <f t="shared" ca="1" si="35"/>
         <v/>
@@ -7306,7 +7307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H105" s="1" t="str">
         <f t="shared" ca="1" si="35"/>
         <v/>
@@ -7328,7 +7329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H106" s="1" t="str">
         <f t="shared" ca="1" si="35"/>
         <v/>
@@ -7350,7 +7351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H107" s="1" t="str">
         <f t="shared" ca="1" si="35"/>
         <v/>
@@ -7372,7 +7373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H108" s="1" t="str">
         <f t="shared" ca="1" si="35"/>
         <v/>
@@ -7394,7 +7395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H109" s="1" t="str">
         <f t="shared" ca="1" si="35"/>
         <v/>
@@ -7416,7 +7417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H110" s="1" t="str">
         <f t="shared" ca="1" si="35"/>
         <v/>
@@ -7438,7 +7439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H111" s="1" t="str">
         <f t="shared" ca="1" si="35"/>
         <v/>
@@ -7460,7 +7461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H112" s="1" t="str">
         <f t="shared" ca="1" si="35"/>
         <v/>
@@ -7482,7 +7483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H113" s="1" t="str">
         <f t="shared" ca="1" si="35"/>
         <v/>
@@ -7504,7 +7505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H114" s="1" t="str">
         <f t="shared" ca="1" si="35"/>
         <v/>
@@ -7526,7 +7527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H115" s="1" t="str">
         <f t="shared" ca="1" si="35"/>
         <v/>
@@ -7548,7 +7549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H116" s="1" t="str">
         <f t="shared" ca="1" si="35"/>
         <v/>
@@ -7570,7 +7571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H117" s="1" t="str">
         <f t="shared" ca="1" si="35"/>
         <v/>
@@ -7592,7 +7593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H118" s="1" t="str">
         <f t="shared" ca="1" si="35"/>
         <v/>
@@ -7614,7 +7615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H119" s="1" t="str">
         <f t="shared" ca="1" si="35"/>
         <v/>
@@ -7636,7 +7637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H120" s="1" t="str">
         <f t="shared" ca="1" si="35"/>
         <v/>
@@ -7658,7 +7659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H121" s="1" t="str">
         <f t="shared" ca="1" si="35"/>
         <v/>
@@ -7680,7 +7681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H122" s="1" t="str">
         <f t="shared" ca="1" si="35"/>
         <v/>
@@ -7702,7 +7703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="8:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="8:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H123" s="1" t="str">
         <f t="shared" ca="1" si="35"/>
         <v/>
@@ -7760,7 +7761,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>'Соль SKU'!$A$1:$A$137</xm:f>
           </x14:formula1>
@@ -7776,148 +7777,148 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMK27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.6328125" style="1" customWidth="1"/>
-    <col min="2" max="1025" width="8.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="43.6640625" style="1" customWidth="1"/>
+    <col min="2" max="1025" width="8.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="6" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>13</v>
       </c>
@@ -7929,162 +7930,162 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMK29"/>
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.7265625" style="1" customWidth="1"/>
-    <col min="2" max="1025" width="8.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="43.77734375" style="1" customWidth="1"/>
+    <col min="2" max="1025" width="8.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="6" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="6" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="6" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" s="6" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added full cleaning before non-lactose boiling
</commit_message>
<xml_diff>
--- a/app/schedule_maker/data/sample_boiling_plan.xlsx
+++ b/app/schedule_maker/data/sample_boiling_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mi\Desktop\code\git\2020.10-umalat\umalat\app\schedule_maker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5438B778-C454-44F1-A87E-5ACD538529A7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6AFE75-5A9E-4539-83BE-69607C864EF9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="76">
   <si>
     <t>Номер партии</t>
   </si>
@@ -251,6 +251,9 @@
   </si>
   <si>
     <t xml:space="preserve">3.6, Альче </t>
+  </si>
+  <si>
+    <t>2.7, Альче, без лактозы</t>
   </si>
 </sst>
 </file>
@@ -4178,7 +4181,7 @@
       <pane xSplit="13" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="N1" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4644,7 +4647,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D10" s="14">
         <v>850</v>
@@ -4653,7 +4656,7 @@
         <v>30</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="G10" s="14">
         <v>850</v>

</xml_diff>